<commit_message>
Cập nhật nhiệm vụ của Dũng trong Bảng phân công công việc
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\Thuc tap nhom\Final\Quan ly khach san\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\GITHUB\QLKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,9 +59,6 @@
     <t>Xây dựng module quản lý nhân viên, khách hàng</t>
   </si>
   <si>
-    <t>Xây dựng tài liệu hướng dẫn cài đặt, vận hành</t>
-  </si>
-  <si>
     <t>Tú</t>
   </si>
   <si>
@@ -74,13 +71,16 @@
     <t>Lập</t>
   </si>
   <si>
-    <t>SinnaSone</t>
-  </si>
-  <si>
     <t>Dũng</t>
   </si>
   <si>
     <t>Thiết kế giao diện đăng nhập, màn hình chính, giới thiệu.</t>
+  </si>
+  <si>
+    <t>Sinna Sone</t>
+  </si>
+  <si>
+    <t>Xây dựng README.md, LICENSE</t>
   </si>
 </sst>
 </file>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +509,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="6"/>
     </row>
@@ -518,10 +518,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6"/>
     </row>
@@ -533,7 +533,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6"/>
     </row>
@@ -545,7 +545,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -557,7 +557,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -569,7 +569,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -581,19 +581,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" s="7"/>
     </row>

</xml_diff>

<commit_message>
Cập nhật lại phân công công việc, ghép công việc Lập Tuấn
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -68,9 +68,6 @@
     <t>Phát</t>
   </si>
   <si>
-    <t>Lập</t>
-  </si>
-  <si>
     <t>Dũng</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Xây dựng README.md, LICENSE</t>
+  </si>
+  <si>
+    <t>Lập, Tuấn</t>
   </si>
 </sst>
 </file>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>11</v>
@@ -557,7 +557,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -581,7 +581,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="6"/>
     </row>
@@ -590,10 +590,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="7"/>
     </row>

</xml_diff>